<commit_message>
Enable non-class style notation for TypeScript.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgClassValueObject.xlsx
+++ b/meta/program/BlancoCgClassValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A729184-79B9-644C-AD0E-4F15A0872A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28827FBC-F15F-7043-9E32-ECC3221F8417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21140" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -429,6 +429,24 @@
     </rPh>
     <rPh sb="42" eb="44">
       <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>noClassDeclare</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>trueの場合、クラス宣言を省略します。</t>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">バアイ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ショウリャク </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -436,7 +454,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -926,43 +944,43 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1278,14 +1296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E41" sqref="E41:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1352,12 +1370,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1458,23 +1476,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="51"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="51"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1511,29 +1529,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="44" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="33.75" customHeight="1">
@@ -1547,10 +1565,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="20"/>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="56"/>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" spans="1:6" ht="29.25" customHeight="1">
       <c r="A28" s="21">
@@ -1564,10 +1582,10 @@
         <v>46</v>
       </c>
       <c r="D28" s="23"/>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="48"/>
+      <c r="F28" s="46"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="21">
@@ -1600,10 +1618,10 @@
       <c r="D30" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="48"/>
+      <c r="F30" s="46"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="21">
@@ -1638,10 +1656,10 @@
       <c r="D32" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="47" t="s">
+      <c r="E32" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="46"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="21">
@@ -1694,10 +1712,10 @@
       <c r="D35" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="48"/>
+      <c r="F35" s="46"/>
     </row>
     <row r="36" spans="1:6" ht="29.25" customHeight="1">
       <c r="A36" s="21">
@@ -1712,10 +1730,10 @@
       <c r="D36" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="48"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="21">
@@ -1776,10 +1794,18 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="B40" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>86</v>
+      </c>
       <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" ht="44.25" customHeight="1">
@@ -1794,10 +1820,10 @@
         <v>48</v>
       </c>
       <c r="D41" s="23"/>
-      <c r="E41" s="47" t="s">
+      <c r="E41" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="48"/>
+      <c r="F41" s="46"/>
     </row>
     <row r="42" spans="1:6" ht="35" customHeight="1">
       <c r="A42" s="21">
@@ -1813,10 +1839,10 @@
       <c r="D42" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="47" t="s">
+      <c r="E42" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="48"/>
+      <c r="F42" s="46"/>
     </row>
     <row r="43" spans="1:6" ht="35" customHeight="1">
       <c r="A43" s="21">
@@ -1832,10 +1858,10 @@
       <c r="D43" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="48"/>
+      <c r="F43" s="46"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="25"/>
@@ -1847,6 +1873,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="D25:D26"/>
@@ -1857,11 +1888,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E30:F30"/>
@@ -1870,23 +1896,23 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D60">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D60" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1899,7 +1925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
3.0.7: Support JsonCreator annotation for kotlin primary constructor.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgClassValueObject.xlsx
+++ b/meta/program/BlancoCgClassValueObject.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28827FBC-F15F-7043-9E32-ECC3221F8417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC4211A-55E2-1349-A6DD-F7961CFFF18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21140" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="89">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -447,6 +447,17 @@
     </rPh>
     <rPh sb="14" eb="16">
       <t xml:space="preserve">ショウリャク </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>jsonCreator</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>primary constructor に JsonCreator アノテーションを付与します。</t>
+    <rPh sb="42" eb="44">
+      <t xml:space="preserve">フヨシマス。 </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -831,16 +842,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,11 +950,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,9 +971,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -965,7 +980,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -973,12 +988,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1300,10 +1309,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:F41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1319,7 +1328,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1342,31 +1351,31 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="57" customHeight="1">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
@@ -1378,11 +1387,11 @@
       <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="35" t="s">
         <v>27</v>
       </c>
       <c r="D9"/>
@@ -1390,21 +1399,21 @@
       <c r="F9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="35"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D11"/>
@@ -1412,11 +1421,11 @@
       <c r="F11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="36" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D12"/>
@@ -1424,21 +1433,21 @@
       <c r="F12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="36"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="35"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
@@ -1450,435 +1459,449 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="51"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="51"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="40"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="39"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="25"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="41"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="40"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="52" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="53"/>
     </row>
     <row r="28" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <f>A27+1</f>
         <v>2</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="56" t="s">
+      <c r="D28" s="22"/>
+      <c r="E28" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="46"/>
+      <c r="F28" s="47"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="21">
-        <f t="shared" ref="A29:A43" si="0">A28+1</f>
+      <c r="A29" s="20">
+        <f t="shared" ref="A29:A44" si="0">A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="46"/>
+      <c r="F30" s="47"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="21">
+      <c r="A31" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="24"/>
+      <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" ht="45" customHeight="1">
-      <c r="A32" s="21">
+      <c r="A32" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="46"/>
+      <c r="F32" s="47"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="21">
+      <c r="A33" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="24"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="21">
+      <c r="A34" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="24"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" ht="42" customHeight="1">
-      <c r="A35" s="21">
+      <c r="A35" s="20">
         <v>9</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="43" t="s">
+      <c r="D35" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="46"/>
+      <c r="F35" s="47"/>
     </row>
     <row r="36" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A36" s="21">
+      <c r="A36" s="20">
         <v>10</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="E36" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="46"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="21">
+      <c r="A37" s="20">
         <v>11</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="24"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="21">
+      <c r="A38" s="20">
         <v>12</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="24"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="21">
+      <c r="A39" s="20">
         <v>13</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="24"/>
+      <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="21">
+      <c r="A40" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="23" t="b">
+      <c r="D40" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="24"/>
+      <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" ht="44.25" customHeight="1">
-      <c r="A41" s="21">
+      <c r="A41" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="45" t="s">
+      <c r="D41" s="22"/>
+      <c r="E41" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="46"/>
+      <c r="F41" s="47"/>
     </row>
     <row r="42" spans="1:6" ht="35" customHeight="1">
-      <c r="A42" s="21">
+      <c r="A42" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="46"/>
+      <c r="F42" s="47"/>
     </row>
     <row r="43" spans="1:6" ht="35" customHeight="1">
-      <c r="A43" s="21">
+      <c r="A43" s="20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="46"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="25"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
+      <c r="F43" s="47"/>
+    </row>
+    <row r="44" spans="1:6" ht="35" customHeight="1">
+      <c r="A44" s="20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="47"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
+  <mergeCells count="21">
+    <mergeCell ref="E44:F44"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="D19:D20"/>
@@ -1893,10 +1916,16 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D60" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1957,54 +1986,54 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="32"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="37"/>
-      <c r="D4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="36"/>
+      <c r="D4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>